<commit_message>
creating master db with ableist and suggestion words
</commit_message>
<xml_diff>
--- a/master_db.xlsx
+++ b/master_db.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaitanyakunapareddi/Desktop/iconsult/ad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF871A23-91F6-7E42-94A0-896AFF6CD432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D28B0E-3A9F-CD48-89BC-622D1495EB91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15320" xr2:uid="{481C1F8F-F1C7-AC46-B12E-AB44130B1BFA}"/>
   </bookViews>
   <sheets>
-    <sheet name="ablesit" sheetId="1" r:id="rId1"/>
+    <sheet name="ableist" sheetId="1" r:id="rId1"/>
     <sheet name="suggestions" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,6 +32,377 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
+  <si>
+    <t>autistic</t>
+  </si>
+  <si>
+    <t>dense</t>
+  </si>
+  <si>
+    <t>Ignorant</t>
+  </si>
+  <si>
+    <t>Bizarre</t>
+  </si>
+  <si>
+    <t>outrageous</t>
+  </si>
+  <si>
+    <t>deaf and mute</t>
+  </si>
+  <si>
+    <t>mentally deranged</t>
+  </si>
+  <si>
+    <t>epileptic seizure.</t>
+  </si>
+  <si>
+    <t>gimpy </t>
+  </si>
+  <si>
+    <t>mentally deficient</t>
+  </si>
+  <si>
+    <t>can’t talk</t>
+  </si>
+  <si>
+    <t>able-bodied</t>
+  </si>
+  <si>
+    <t>abnormal</t>
+  </si>
+  <si>
+    <t>addict</t>
+  </si>
+  <si>
+    <t>afflicted</t>
+  </si>
+  <si>
+    <t>attention-seeking</t>
+  </si>
+  <si>
+    <t>autism </t>
+  </si>
+  <si>
+    <t>batty</t>
+  </si>
+  <si>
+    <t>birth defect</t>
+  </si>
+  <si>
+    <t>blind</t>
+  </si>
+  <si>
+    <t>bonkers</t>
+  </si>
+  <si>
+    <t>brain damaged</t>
+  </si>
+  <si>
+    <t>challenged</t>
+  </si>
+  <si>
+    <t>crazy</t>
+  </si>
+  <si>
+    <t>cretin</t>
+  </si>
+  <si>
+    <t>cripple </t>
+  </si>
+  <si>
+    <t>confined to a wheelchair</t>
+  </si>
+  <si>
+    <t>daft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deaf and dumb </t>
+  </si>
+  <si>
+    <t>defect</t>
+  </si>
+  <si>
+    <t>deformed</t>
+  </si>
+  <si>
+    <t>delusional</t>
+  </si>
+  <si>
+    <t>demented</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deranged </t>
+  </si>
+  <si>
+    <t>derp</t>
+  </si>
+  <si>
+    <t>differently abled</t>
+  </si>
+  <si>
+    <t>dim </t>
+  </si>
+  <si>
+    <t>disorder</t>
+  </si>
+  <si>
+    <t>dotard</t>
+  </si>
+  <si>
+    <t>dumb</t>
+  </si>
+  <si>
+    <t>dwarf</t>
+  </si>
+  <si>
+    <t>epileptic</t>
+  </si>
+  <si>
+    <t>exceptional</t>
+  </si>
+  <si>
+    <t>feeble-minded</t>
+  </si>
+  <si>
+    <t>flid</t>
+  </si>
+  <si>
+    <t>freak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gimp </t>
+  </si>
+  <si>
+    <t>handicapped</t>
+  </si>
+  <si>
+    <t>handicapable</t>
+  </si>
+  <si>
+    <t>hare lip</t>
+  </si>
+  <si>
+    <t>hearing-impaired</t>
+  </si>
+  <si>
+    <t>homebound</t>
+  </si>
+  <si>
+    <t>hyper</t>
+  </si>
+  <si>
+    <t>hyper-sensitive</t>
+  </si>
+  <si>
+    <t>hysterical</t>
+  </si>
+  <si>
+    <t>imbecile was the diagnostic term</t>
+  </si>
+  <si>
+    <t>incapacitated</t>
+  </si>
+  <si>
+    <t>idiot </t>
+  </si>
+  <si>
+    <t xml:space="preserve">inmate </t>
+  </si>
+  <si>
+    <t>insane</t>
+  </si>
+  <si>
+    <t>inspirational</t>
+  </si>
+  <si>
+    <t>invalid</t>
+  </si>
+  <si>
+    <t>junkie</t>
+  </si>
+  <si>
+    <t>lame</t>
+  </si>
+  <si>
+    <t>losing one's mind</t>
+  </si>
+  <si>
+    <t>likely to become a public charge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lunatic </t>
+  </si>
+  <si>
+    <t>mad</t>
+  </si>
+  <si>
+    <t>maniac</t>
+  </si>
+  <si>
+    <t>midget</t>
+  </si>
+  <si>
+    <t>mong</t>
+  </si>
+  <si>
+    <t>moron</t>
+  </si>
+  <si>
+    <t>mute</t>
+  </si>
+  <si>
+    <t>mutant</t>
+  </si>
+  <si>
+    <t>narc</t>
+  </si>
+  <si>
+    <t>nut</t>
+  </si>
+  <si>
+    <t>paraplegic</t>
+  </si>
+  <si>
+    <t>psychopath</t>
+  </si>
+  <si>
+    <t>scatterbrained</t>
+  </si>
+  <si>
+    <t>schizo </t>
+  </si>
+  <si>
+    <t>schizophrenic</t>
+  </si>
+  <si>
+    <t>senile</t>
+  </si>
+  <si>
+    <t>slow</t>
+  </si>
+  <si>
+    <t>sluggish</t>
+  </si>
+  <si>
+    <t>sociopath</t>
+  </si>
+  <si>
+    <t>spastic</t>
+  </si>
+  <si>
+    <t>special</t>
+  </si>
+  <si>
+    <t>special needs</t>
+  </si>
+  <si>
+    <t>stone deaf</t>
+  </si>
+  <si>
+    <t>stricken</t>
+  </si>
+  <si>
+    <t>subnormal</t>
+  </si>
+  <si>
+    <t>supercrip</t>
+  </si>
+  <si>
+    <t>sufferer</t>
+  </si>
+  <si>
+    <t>tard</t>
+  </si>
+  <si>
+    <t>thick</t>
+  </si>
+  <si>
+    <t>tone deaf</t>
+  </si>
+  <si>
+    <t>unclean</t>
+  </si>
+  <si>
+    <t>unfortunate</t>
+  </si>
+  <si>
+    <t>wheelchair bound</t>
+  </si>
+  <si>
+    <t>is non-verbal</t>
+  </si>
+  <si>
+    <t>barren</t>
+  </si>
+  <si>
+    <t>cripple</t>
+  </si>
+  <si>
+    <t>harelip</t>
+  </si>
+  <si>
+    <t>mongoloid</t>
+  </si>
+  <si>
+    <t>bipolar</t>
+  </si>
+  <si>
+    <t>schizo</t>
+  </si>
+  <si>
+    <t>abuser</t>
+  </si>
+  <si>
+    <t>is mentally ill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is emotionally </t>
+  </si>
+  <si>
+    <t>is insane</t>
+  </si>
+  <si>
+    <t>nuts</t>
+  </si>
+  <si>
+    <t>wacko</t>
+  </si>
+  <si>
+    <t>slow learner</t>
+  </si>
+  <si>
+    <t>special education student</t>
+  </si>
+  <si>
+    <t>stroke victim</t>
+  </si>
+  <si>
+    <t>person afflicted with epilepsy</t>
+  </si>
+  <si>
+    <t>burn victim</t>
+  </si>
+  <si>
+    <t>handicapped parking</t>
+  </si>
+  <si>
+    <t>disabled restroom</t>
+  </si>
+  <si>
+    <t>unsuccessful suicide</t>
+  </si>
+  <si>
+    <t>committed suicide</t>
+  </si>
+  <si>
+    <t>mental health patient</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -65,8 +436,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,24 +753,664 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB4188E-3C18-A845-AC24-A1EAE0080528}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A102" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A104" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A105" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A106" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A107" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A108" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A109" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A110" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A111" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A112" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A113" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A114" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A115" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A116" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A117" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A118" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A119"/>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A120"/>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A121"/>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A122"/>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A123"/>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A124"/>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A125"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{622F424A-2A3F-BA4D-B876-164279C63F0D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>